<commit_message>
adding basic information to gantt chart
</commit_message>
<xml_diff>
--- a/Documentation/SprintPlans/GanttChart.xlsx
+++ b/Documentation/SprintPlans/GanttChart.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3026F0BE-129B-4444-AC61-3ACF781B445C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822AF429-8657-4028-8BBB-2AF8D251E7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>ABOUT THIS GANTT CHART</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Assigned to</t>
-  </si>
-  <si>
     <t>Progress</t>
   </si>
   <si>
@@ -95,97 +92,10 @@
     <t>Days</t>
   </si>
   <si>
-    <t>Project development</t>
-  </si>
-  <si>
-    <t>Project charter</t>
-  </si>
-  <si>
-    <t>Goal</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Research</t>
-  </si>
-  <si>
-    <t>Milestone</t>
-  </si>
-  <si>
-    <t>Projections</t>
-  </si>
-  <si>
     <t>Low Risk</t>
   </si>
   <si>
-    <t>Stakeholders</t>
-  </si>
-  <si>
-    <t>Review</t>
-  </si>
-  <si>
-    <t>Med Risk</t>
-  </si>
-  <si>
-    <t>Contracts</t>
-  </si>
-  <si>
-    <t>Proposals</t>
-  </si>
-  <si>
-    <t>High Risk</t>
-  </si>
-  <si>
-    <t>Document review</t>
-  </si>
-  <si>
     <t>On Track</t>
-  </si>
-  <si>
-    <t>Bid date</t>
-  </si>
-  <si>
-    <t>Award date</t>
-  </si>
-  <si>
-    <t>Finalize</t>
-  </si>
-  <si>
-    <t>Design</t>
-  </si>
-  <si>
-    <t>Feasibility study</t>
-  </si>
-  <si>
-    <t>Submit permit applications</t>
-  </si>
-  <si>
-    <t>Design proposal</t>
-  </si>
-  <si>
-    <t>Materials</t>
-  </si>
-  <si>
-    <t>Equipment</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Environment</t>
-  </si>
-  <si>
-    <t>System test</t>
-  </si>
-  <si>
-    <t>Issues/bugs</t>
-  </si>
-  <si>
-    <t>Task 4</t>
-  </si>
-  <si>
-    <t>Task 5</t>
   </si>
   <si>
     <t>To add more data, Insert new rows ABOVE this one</t>
@@ -195,6 +105,66 @@
   </si>
   <si>
     <t>COMP3000</t>
+  </si>
+  <si>
+    <t>Project Planning</t>
+  </si>
+  <si>
+    <t>Development phase 1: MVP</t>
+  </si>
+  <si>
+    <t>Development Phase 2: footprint calculation</t>
+  </si>
+  <si>
+    <t>Project Initiation</t>
+  </si>
+  <si>
+    <t>requirements abstraction and user story mapping</t>
+  </si>
+  <si>
+    <t>Legal, Social, Ethical and Professional considerations</t>
+  </si>
+  <si>
+    <t>Basic GUI creation in Python</t>
+  </si>
+  <si>
+    <t>research and shortlist of OSINT tools to implement</t>
+  </si>
+  <si>
+    <t>Low fidelity prototyping</t>
+  </si>
+  <si>
+    <t>implementation of basic OSINT api's</t>
+  </si>
+  <si>
+    <t>Displaying OSINT harvested data to the user</t>
+  </si>
+  <si>
+    <t>implementing hardcoded tips section</t>
+  </si>
+  <si>
+    <t>Bug fixing</t>
+  </si>
+  <si>
+    <t>Development Phase 4: Ensuring Legal and ethical compliance</t>
+  </si>
+  <si>
+    <t>Development Phase 3: accounts and footprint score persistence</t>
+  </si>
+  <si>
+    <t>Development Phase 5: Final product development</t>
+  </si>
+  <si>
+    <t>unit Testing</t>
+  </si>
+  <si>
+    <t>User acceptance Testing</t>
+  </si>
+  <si>
+    <t>Assigned to(Harry)</t>
+  </si>
+  <si>
+    <t>Sprint Overrun</t>
   </si>
 </sst>
 </file>
@@ -661,7 +631,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -882,6 +852,12 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -1609,8 +1585,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Milestones4352" displayName="Milestones4352" ref="B9:G36" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="B9:G36" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Milestones4352" displayName="Milestones4352" ref="B9:G37" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="B9:G37" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1621,7 +1597,7 @@
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{619BF8F6-D0F1-41AD-871D-FE0240C45A93}" name="Milestone description" dataDxfId="19"/>
     <tableColumn id="2" xr3:uid="{39BD914E-FB02-4352-846C-6D59624DC0B0}" name="Category" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{D274194F-BCA0-44F3-84B2-217254EE241C}" name="Assigned to" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{D274194F-BCA0-44F3-84B2-217254EE241C}" name="Assigned to(Harry)" dataDxfId="17"/>
     <tableColumn id="4" xr3:uid="{8385BC6F-56EE-4363-A106-8DB0A1E4EF5A}" name="Progress" dataDxfId="16"/>
     <tableColumn id="5" xr3:uid="{02926609-7B93-4B6F-BE96-92EC7A949E4B}" name="Start" dataDxfId="15" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{8FF9BE8E-04B7-4B39-AC27-D2E534204BC3}" name="Days" dataDxfId="14" dataCellStyle="Comma [0]"/>
@@ -2071,10 +2047,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BP38"/>
+  <dimension ref="A1:BP39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="38" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="62" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2095,7 +2071,7 @@
     <row r="2" spans="1:68" ht="49.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="77" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C2" s="77"/>
       <c r="D2" s="77"/>
@@ -2220,7 +2196,7 @@
     <row r="5" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10"/>
       <c r="B5" s="72" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="C5" s="32"/>
       <c r="D5" s="32"/>
@@ -2636,16 +2612,16 @@
         <v>12</v>
       </c>
       <c r="D9" s="68" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="68" t="s">
+      <c r="F9" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="68" t="s">
+      <c r="G9" s="68" t="s">
         <v>15</v>
-      </c>
-      <c r="G9" s="68" t="s">
-        <v>16</v>
       </c>
       <c r="H9" s="45"/>
       <c r="I9" s="59" t="str">
@@ -2940,7 +2916,7 @@
     <row r="11" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10"/>
       <c r="B11" s="70" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
@@ -2949,7 +2925,7 @@
       <c r="G11" s="23"/>
       <c r="H11" s="20"/>
       <c r="I11" s="17" t="str">
-        <f t="shared" ref="I11:X26" ca="1" si="4">IF(AND($C11="Goal",I$7&gt;=$F11,I$7&lt;=$F11+$G11-1),2,IF(AND($C11="Milestone",I$7&gt;=$F11,I$7&lt;=$F11+$G11-1),1,""))</f>
+        <f t="shared" ref="I11:X27" ca="1" si="4">IF(AND($C11="Goal",I$7&gt;=$F11,I$7&lt;=$F11+$G11-1),2,IF(AND($C11="Milestone",I$7&gt;=$F11,I$7&lt;=$F11+$G11-1),1,""))</f>
         <v/>
       </c>
       <c r="J11" s="17" t="str">
@@ -3013,7 +2989,7 @@
         <v/>
       </c>
       <c r="Y11" s="17" t="str">
-        <f t="shared" ref="Y11:AN26" ca="1" si="5">IF(AND($C11="Goal",Y$7&gt;=$F11,Y$7&lt;=$F11+$G11-1),2,IF(AND($C11="Milestone",Y$7&gt;=$F11,Y$7&lt;=$F11+$G11-1),1,""))</f>
+        <f t="shared" ref="Y11:AN27" ca="1" si="5">IF(AND($C11="Goal",Y$7&gt;=$F11,Y$7&lt;=$F11+$G11-1),2,IF(AND($C11="Milestone",Y$7&gt;=$F11,Y$7&lt;=$F11+$G11-1),1,""))</f>
         <v/>
       </c>
       <c r="Z11" s="17" t="str">
@@ -3077,7 +3053,7 @@
         <v/>
       </c>
       <c r="AO11" s="17" t="str">
-        <f t="shared" ref="AO11:BD26" ca="1" si="6">IF(AND($C11="Goal",AO$7&gt;=$F11,AO$7&lt;=$F11+$G11-1),2,IF(AND($C11="Milestone",AO$7&gt;=$F11,AO$7&lt;=$F11+$G11-1),1,""))</f>
+        <f t="shared" ref="AO11:BD27" ca="1" si="6">IF(AND($C11="Goal",AO$7&gt;=$F11,AO$7&lt;=$F11+$G11-1),2,IF(AND($C11="Milestone",AO$7&gt;=$F11,AO$7&lt;=$F11+$G11-1),1,""))</f>
         <v/>
       </c>
       <c r="AP11" s="17" t="str">
@@ -3141,7 +3117,7 @@
         <v/>
       </c>
       <c r="BE11" s="17" t="str">
-        <f t="shared" ref="BE11:BL26" ca="1" si="7">IF(AND($C11="Goal",BE$7&gt;=$F11,BE$7&lt;=$F11+$G11-1),2,IF(AND($C11="Milestone",BE$7&gt;=$F11,BE$7&lt;=$F11+$G11-1),1,""))</f>
+        <f t="shared" ref="BE11:BL27" ca="1" si="7">IF(AND($C11="Goal",BE$7&gt;=$F11,BE$7&lt;=$F11+$G11-1),2,IF(AND($C11="Milestone",BE$7&gt;=$F11,BE$7&lt;=$F11+$G11-1),1,""))</f>
         <v/>
       </c>
       <c r="BF11" s="17" t="str">
@@ -3177,23 +3153,21 @@
     <row r="12" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10"/>
       <c r="B12" s="71" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>20</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D12" s="20"/>
       <c r="E12" s="21">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="F12" s="22">
         <f ca="1">TODAY()</f>
-        <v>45565</v>
+        <v>45573</v>
       </c>
       <c r="G12" s="23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H12" s="20"/>
       <c r="I12" s="17" t="str">
@@ -3424,24 +3398,26 @@
     <row r="13" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10"/>
       <c r="B13" s="71" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D13" s="20"/>
-      <c r="E13" s="21"/>
+      <c r="E13" s="21">
+        <v>0</v>
+      </c>
       <c r="F13" s="22">
         <f ca="1">TODAY()+5</f>
-        <v>45570</v>
+        <v>45578</v>
       </c>
       <c r="G13" s="23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H13" s="20"/>
-      <c r="I13" s="17">
-        <f t="shared" ref="I13:X28" ca="1" si="8">IF(AND($C13="Goal",I$7&gt;=$F13,I$7&lt;=$F13+$G13-1),2,IF(AND($C13="Milestone",I$7&gt;=$F13,I$7&lt;=$F13+$G13-1),1,""))</f>
-        <v>1</v>
+      <c r="I13" s="17" t="str">
+        <f t="shared" ref="I13:X29" ca="1" si="8">IF(AND($C13="Goal",I$7&gt;=$F13,I$7&lt;=$F13+$G13-1),2,IF(AND($C13="Milestone",I$7&gt;=$F13,I$7&lt;=$F13+$G13-1),1,""))</f>
+        <v/>
       </c>
       <c r="J13" s="17" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -3667,21 +3643,21 @@
     <row r="14" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
       <c r="B14" s="71" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="21">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F14" s="22">
-        <f ca="1">F12-3</f>
-        <v>45562</v>
+        <f ca="1">F13+8</f>
+        <v>45586</v>
       </c>
       <c r="G14" s="23">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="17" t="str">
@@ -3912,19 +3888,21 @@
     <row r="15" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="B15" s="71" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
+      <c r="E15" s="21">
+        <v>0</v>
+      </c>
       <c r="F15" s="22">
-        <f ca="1">F12+20</f>
-        <v>45585</v>
+        <f ca="1">F14+2</f>
+        <v>45588</v>
       </c>
       <c r="G15" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15" s="20"/>
       <c r="I15" s="17" t="str">
@@ -3987,9 +3965,9 @@
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="X15" s="17">
-        <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+      <c r="X15" s="17" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
       <c r="Y15" s="17" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4155,21 +4133,21 @@
     <row r="16" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="71" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="22">
-        <f ca="1">F12+6</f>
-        <v>45571</v>
+        <f ca="1">F15+ 5</f>
+        <v>45593</v>
       </c>
       <c r="G16" s="23">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H16" s="20"/>
       <c r="I16" s="17" t="str">
@@ -4400,7 +4378,7 @@
     <row r="17" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10"/>
       <c r="B17" s="70" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
@@ -4636,21 +4614,20 @@
     <row r="18" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10"/>
       <c r="B18" s="71" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="21">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="F18" s="22">
-        <f ca="1">F12+6</f>
-        <v>45571</v>
+        <v>45600</v>
       </c>
       <c r="G18" s="23">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H18" s="20"/>
       <c r="I18" s="17" t="str">
@@ -4881,21 +4858,21 @@
     <row r="19" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
       <c r="B19" s="71" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="21">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F19" s="22">
-        <f ca="1">F18+2</f>
-        <v>45573</v>
+        <f>F18+7</f>
+        <v>45607</v>
       </c>
       <c r="G19" s="23">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H19" s="20"/>
       <c r="I19" s="17" t="str">
@@ -5126,21 +5103,21 @@
     <row r="20" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
       <c r="B20" s="71" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="21">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="F20" s="22">
-        <f ca="1">F19+5</f>
-        <v>45578</v>
+        <f>F19+5</f>
+        <v>45612</v>
       </c>
       <c r="G20" s="23">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H20" s="20"/>
       <c r="I20" s="17" t="str">
@@ -5371,19 +5348,21 @@
     <row r="21" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9"/>
       <c r="B21" s="71" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D21" s="20"/>
-      <c r="E21" s="21"/>
+      <c r="E21" s="21">
+        <v>0</v>
+      </c>
       <c r="F21" s="22">
-        <f ca="1">F20+2</f>
-        <v>45580</v>
+        <f>F20+16</f>
+        <v>45628</v>
       </c>
       <c r="G21" s="23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="17" t="str">
@@ -5426,9 +5405,9 @@
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="S21" s="17">
-        <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+      <c r="S21" s="17" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
       <c r="T21" s="17" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -5614,17 +5593,21 @@
     <row r="22" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="B22" s="71" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="20"/>
+        <v>33</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
+      <c r="E22" s="21">
+        <v>0</v>
+      </c>
       <c r="F22" s="22">
-        <f ca="1">F21+1</f>
-        <v>45581</v>
+        <f>F21+3</f>
+        <v>45631</v>
       </c>
       <c r="G22" s="23">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="17" t="str">
@@ -5854,257 +5837,91 @@
     </row>
     <row r="23" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
-      <c r="B23" s="70" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="20"/>
+      <c r="B23" s="84" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="D23" s="20"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="23"/>
+      <c r="E23" s="21">
+        <v>0</v>
+      </c>
+      <c r="F23" s="22">
+        <f>F22+4</f>
+        <v>45635</v>
+      </c>
+      <c r="G23" s="23">
+        <v>5</v>
+      </c>
       <c r="H23" s="20"/>
-      <c r="I23" s="17" t="str">
-        <f t="shared" ca="1" si="8"/>
-        <v/>
-      </c>
-      <c r="J23" s="17" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="K23" s="17" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="L23" s="17" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="M23" s="17" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="N23" s="17" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="O23" s="17" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="P23" s="17" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="Q23" s="17" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="R23" s="17" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="S23" s="17" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="T23" s="17" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="U23" s="17" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="V23" s="17" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="W23" s="17" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="X23" s="17" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="Y23" s="17" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="Z23" s="17" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AA23" s="17" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AB23" s="17" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AC23" s="17" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AD23" s="17" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AE23" s="17" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AF23" s="17" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AG23" s="17" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AH23" s="17" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AI23" s="17" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AJ23" s="17" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AK23" s="17" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AL23" s="17" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AM23" s="17" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AN23" s="17" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AO23" s="17" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AP23" s="17" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AQ23" s="17" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AR23" s="17" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AS23" s="17" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AT23" s="17" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AU23" s="17" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AV23" s="17" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AW23" s="17" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AX23" s="17" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AY23" s="17" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AZ23" s="17" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BA23" s="17" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BB23" s="17" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BC23" s="17" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BD23" s="17" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BE23" s="17" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BF23" s="17" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BG23" s="17" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BH23" s="17" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BI23" s="17" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BJ23" s="17" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BK23" s="17" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BL23" s="17" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17"/>
+      <c r="T23" s="17"/>
+      <c r="U23" s="17"/>
+      <c r="V23" s="17"/>
+      <c r="W23" s="17"/>
+      <c r="X23" s="17"/>
+      <c r="Y23" s="17"/>
+      <c r="Z23" s="17"/>
+      <c r="AA23" s="17"/>
+      <c r="AB23" s="17"/>
+      <c r="AC23" s="17"/>
+      <c r="AD23" s="17"/>
+      <c r="AE23" s="17"/>
+      <c r="AF23" s="17"/>
+      <c r="AG23" s="17"/>
+      <c r="AH23" s="17"/>
+      <c r="AI23" s="17"/>
+      <c r="AJ23" s="17"/>
+      <c r="AK23" s="17"/>
+      <c r="AL23" s="17"/>
+      <c r="AM23" s="17"/>
+      <c r="AN23" s="17"/>
+      <c r="AO23" s="17"/>
+      <c r="AP23" s="17"/>
+      <c r="AQ23" s="17"/>
+      <c r="AR23" s="17"/>
+      <c r="AS23" s="17"/>
+      <c r="AT23" s="17"/>
+      <c r="AU23" s="17"/>
+      <c r="AV23" s="17"/>
+      <c r="AW23" s="17"/>
+      <c r="AX23" s="17"/>
+      <c r="AY23" s="17"/>
+      <c r="AZ23" s="17"/>
+      <c r="BA23" s="17"/>
+      <c r="BB23" s="17"/>
+      <c r="BC23" s="17"/>
+      <c r="BD23" s="17"/>
+      <c r="BE23" s="17"/>
+      <c r="BF23" s="17"/>
+      <c r="BG23" s="17"/>
+      <c r="BH23" s="17"/>
+      <c r="BI23" s="17"/>
+      <c r="BJ23" s="17"/>
+      <c r="BK23" s="17"/>
+      <c r="BL23" s="17"/>
     </row>
     <row r="24" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
-      <c r="B24" s="71" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>32</v>
-      </c>
+      <c r="B24" s="70" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="20"/>
       <c r="D24" s="20"/>
       <c r="E24" s="21"/>
-      <c r="F24" s="22">
-        <f ca="1">F12+15</f>
-        <v>45580</v>
-      </c>
-      <c r="G24" s="23">
-        <v>4</v>
-      </c>
+      <c r="F24" s="22"/>
+      <c r="G24" s="23"/>
       <c r="H24" s="20"/>
       <c r="I24" s="17" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -6331,23 +6148,16 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:64" s="1" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
-      <c r="B25" s="71" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>27</v>
-      </c>
+      <c r="B25" s="70" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="20"/>
       <c r="D25" s="20"/>
       <c r="E25" s="21"/>
-      <c r="F25" s="22">
-        <f ca="1">F24+3</f>
-        <v>45583</v>
-      </c>
-      <c r="G25" s="23">
-        <v>14</v>
-      </c>
+      <c r="F25" s="22"/>
+      <c r="G25" s="23"/>
       <c r="H25" s="20"/>
       <c r="I25" s="17" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -6574,23 +6384,16 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:64" s="1" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
-      <c r="B26" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>32</v>
-      </c>
+      <c r="B26" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="20"/>
       <c r="D26" s="20"/>
       <c r="E26" s="21"/>
-      <c r="F26" s="22">
-        <f ca="1">F25+15</f>
-        <v>45598</v>
-      </c>
-      <c r="G26" s="23">
-        <v>6</v>
-      </c>
+      <c r="F26" s="22"/>
+      <c r="G26" s="23"/>
       <c r="H26" s="20"/>
       <c r="I26" s="17" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -6717,7 +6520,7 @@
         <v/>
       </c>
       <c r="AN26" s="17" t="str">
-        <f t="shared" ref="AN26:BC35" ca="1" si="9">IF(AND($C26="Goal",AN$7&gt;=$F26,AN$7&lt;=$F26+$G26-1),2,IF(AND($C26="Milestone",AN$7&gt;=$F26,AN$7&lt;=$F26+$G26-1),1,""))</f>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AO26" s="17" t="str">
@@ -6781,7 +6584,7 @@
         <v/>
       </c>
       <c r="BD26" s="17" t="str">
-        <f t="shared" ref="BD26:BL35" ca="1" si="10">IF(AND($C26="Goal",BD$7&gt;=$F26,BD$7&lt;=$F26+$G26-1),2,IF(AND($C26="Milestone",BD$7&gt;=$F26,BD$7&lt;=$F26+$G26-1),1,""))</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="BE26" s="17" t="str">
@@ -6817,266 +6620,252 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:64" s="1" customFormat="1" ht="110" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
-      <c r="B27" s="71" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>19</v>
-      </c>
+      <c r="B27" s="70" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="20"/>
       <c r="D27" s="20"/>
       <c r="E27" s="21"/>
-      <c r="F27" s="22">
-        <f ca="1">F21+22</f>
-        <v>45602</v>
-      </c>
-      <c r="G27" s="23">
-        <v>3</v>
-      </c>
+      <c r="F27" s="22"/>
+      <c r="G27" s="23"/>
       <c r="H27" s="20"/>
       <c r="I27" s="17" t="str">
         <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="J27" s="17" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="K27" s="17" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="L27" s="17" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="M27" s="17" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="N27" s="17" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="O27" s="17" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="P27" s="17" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="Q27" s="17" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="R27" s="17" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="S27" s="17" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="T27" s="17" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="U27" s="17" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="V27" s="17" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="W27" s="17" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="X27" s="17" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="Y27" s="17" t="str">
-        <f t="shared" ref="Y27:AM35" ca="1" si="11">IF(AND($C27="Goal",Y$7&gt;=$F27,Y$7&lt;=$F27+$G27-1),2,IF(AND($C27="Milestone",Y$7&gt;=$F27,Y$7&lt;=$F27+$G27-1),1,""))</f>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="Z27" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AA27" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AB27" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AC27" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AD27" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AE27" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AF27" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AG27" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AH27" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AI27" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AJ27" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AK27" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AL27" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AM27" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AN27" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AO27" s="17">
-        <f t="shared" ca="1" si="9"/>
-        <v>2</v>
-      </c>
-      <c r="AP27" s="17">
-        <f t="shared" ca="1" si="9"/>
-        <v>2</v>
-      </c>
-      <c r="AQ27" s="17">
-        <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <f t="shared" ref="AN27:BC36" ca="1" si="9">IF(AND($C27="Goal",AN$7&gt;=$F27,AN$7&lt;=$F27+$G27-1),2,IF(AND($C27="Milestone",AN$7&gt;=$F27,AN$7&lt;=$F27+$G27-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AO27" s="17" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="AP27" s="17" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="AQ27" s="17" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
       </c>
       <c r="AR27" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="AS27" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="AT27" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="AU27" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="AV27" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="AW27" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="AX27" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="AY27" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="AZ27" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="BA27" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="BB27" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="BC27" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="BD27" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="BD27:BL36" ca="1" si="10">IF(AND($C27="Goal",BD$7&gt;=$F27,BD$7&lt;=$F27+$G27-1),2,IF(AND($C27="Milestone",BD$7&gt;=$F27,BD$7&lt;=$F27+$G27-1),1,""))</f>
         <v/>
       </c>
       <c r="BE27" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="BF27" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="BG27" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="BH27" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="BI27" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="BJ27" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="BK27" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="BL27" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
       <c r="B28" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>24</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C28" s="20"/>
       <c r="D28" s="20"/>
       <c r="E28" s="21"/>
-      <c r="F28" s="22">
-        <f ca="1">F16</f>
-        <v>45571</v>
-      </c>
-      <c r="G28" s="23">
-        <v>19</v>
-      </c>
+      <c r="F28" s="22"/>
+      <c r="G28" s="23"/>
       <c r="H28" s="20"/>
       <c r="I28" s="17" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -7143,7 +6932,7 @@
         <v/>
       </c>
       <c r="Y28" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ref="Y28:AM36" ca="1" si="11">IF(AND($C28="Goal",Y$7&gt;=$F28,Y$7&lt;=$F28+$G28-1),2,IF(AND($C28="Milestone",Y$7&gt;=$F28,Y$7&lt;=$F28+$G28-1),1,""))</f>
         <v/>
       </c>
       <c r="Z28" s="17" t="str">
@@ -7305,8 +7094,8 @@
     </row>
     <row r="29" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9"/>
-      <c r="B29" s="70" t="s">
-        <v>42</v>
+      <c r="B29" s="71" t="s">
+        <v>38</v>
       </c>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
@@ -7315,67 +7104,67 @@
       <c r="G29" s="23"/>
       <c r="H29" s="20"/>
       <c r="I29" s="17" t="str">
-        <f t="shared" ref="I29:X35" ca="1" si="12">IF(AND($C29="Goal",I$7&gt;=$F29,I$7&lt;=$F29+$G29-1),2,IF(AND($C29="Milestone",I$7&gt;=$F29,I$7&lt;=$F29+$G29-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="J29" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="K29" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="L29" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="M29" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="N29" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="O29" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="P29" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="Q29" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="R29" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="S29" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="T29" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="U29" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="V29" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="W29" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="X29" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="Y29" s="17" t="str">
@@ -7539,24 +7328,19 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:64" s="1" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
-      <c r="B30" s="71" t="s">
-        <v>43</v>
+      <c r="B30" s="83" t="s">
+        <v>33</v>
       </c>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
       <c r="E30" s="21"/>
-      <c r="F30" s="22">
-        <f ca="1">F27+3</f>
-        <v>45605</v>
-      </c>
-      <c r="G30" s="23">
-        <v>15</v>
-      </c>
+      <c r="F30" s="22"/>
+      <c r="G30" s="23"/>
       <c r="H30" s="20"/>
       <c r="I30" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ref="I30:X36" ca="1" si="12">IF(AND($C30="Goal",I$7&gt;=$F30,I$7&lt;=$F30+$G30-1),2,IF(AND($C30="Milestone",I$7&gt;=$F30,I$7&lt;=$F30+$G30-1),1,""))</f>
         <v/>
       </c>
       <c r="J30" s="17" t="str">
@@ -7782,19 +7566,12 @@
     </row>
     <row r="31" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
-      <c r="B31" s="71" t="s">
-        <v>44</v>
-      </c>
+      <c r="B31" s="71"/>
       <c r="C31" s="20"/>
       <c r="D31" s="20"/>
       <c r="E31" s="21"/>
-      <c r="F31" s="22">
-        <f ca="1">F30+14</f>
-        <v>45619</v>
-      </c>
-      <c r="G31" s="23">
-        <v>5</v>
-      </c>
+      <c r="F31" s="22"/>
+      <c r="G31" s="23"/>
       <c r="H31" s="20"/>
       <c r="I31" s="17" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -8023,21 +7800,12 @@
     </row>
     <row r="32" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
-      <c r="B32" s="71" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>22</v>
-      </c>
+      <c r="B32" s="71"/>
+      <c r="C32" s="20"/>
       <c r="D32" s="20"/>
       <c r="E32" s="21"/>
-      <c r="F32" s="22">
-        <f ca="1">F31+42</f>
-        <v>45661</v>
-      </c>
-      <c r="G32" s="23">
-        <v>1</v>
-      </c>
+      <c r="F32" s="22"/>
+      <c r="G32" s="23"/>
       <c r="H32" s="20"/>
       <c r="I32" s="17" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -8266,9 +8034,7 @@
     </row>
     <row r="33" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
-      <c r="B33" s="71" t="s">
-        <v>46</v>
-      </c>
+      <c r="B33" s="71"/>
       <c r="C33" s="20"/>
       <c r="D33" s="20"/>
       <c r="E33" s="21"/>
@@ -8502,9 +8268,7 @@
     </row>
     <row r="34" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
-      <c r="B34" s="24" t="s">
-        <v>47</v>
-      </c>
+      <c r="B34" s="71"/>
       <c r="C34" s="20"/>
       <c r="D34" s="20"/>
       <c r="E34" s="21"/>
@@ -8969,83 +8733,317 @@
         <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
-      <c r="BM35" s="46"/>
     </row>
     <row r="36" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="10"/>
-      <c r="B36" s="69" t="s">
-        <v>48</v>
-      </c>
+      <c r="A36" s="9"/>
+      <c r="B36" s="24"/>
       <c r="C36" s="20"/>
       <c r="D36" s="20"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="43"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="23"/>
       <c r="H36" s="20"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="44"/>
-      <c r="K36" s="44"/>
-      <c r="L36" s="44"/>
-      <c r="M36" s="44"/>
-      <c r="N36" s="44"/>
-      <c r="O36" s="44"/>
-      <c r="P36" s="44"/>
-      <c r="Q36" s="44"/>
-      <c r="R36" s="44"/>
-      <c r="S36" s="44"/>
-      <c r="T36" s="44"/>
-      <c r="U36" s="44"/>
-      <c r="V36" s="44"/>
-      <c r="W36" s="44"/>
-      <c r="X36" s="44"/>
-      <c r="Y36" s="44"/>
-      <c r="Z36" s="44"/>
-      <c r="AA36" s="44"/>
-      <c r="AB36" s="44"/>
-      <c r="AC36" s="44"/>
-      <c r="AD36" s="44"/>
-      <c r="AE36" s="44"/>
-      <c r="AF36" s="44"/>
-      <c r="AG36" s="44"/>
-      <c r="AH36" s="44"/>
-      <c r="AI36" s="44"/>
-      <c r="AJ36" s="44"/>
-      <c r="AK36" s="44"/>
-      <c r="AL36" s="44"/>
-      <c r="AM36" s="44"/>
-      <c r="AN36" s="44"/>
-      <c r="AO36" s="44"/>
-      <c r="AP36" s="44"/>
-      <c r="AQ36" s="44"/>
-      <c r="AR36" s="44"/>
-      <c r="AS36" s="44"/>
-      <c r="AT36" s="44"/>
-      <c r="AU36" s="44"/>
-      <c r="AV36" s="44"/>
-      <c r="AW36" s="44"/>
-      <c r="AX36" s="44"/>
-      <c r="AY36" s="44"/>
-      <c r="AZ36" s="44"/>
-      <c r="BA36" s="44"/>
-      <c r="BB36" s="44"/>
-      <c r="BC36" s="44"/>
-      <c r="BD36" s="44"/>
-      <c r="BE36" s="44"/>
-      <c r="BF36" s="44"/>
-      <c r="BG36" s="44"/>
-      <c r="BH36" s="44"/>
-      <c r="BI36" s="44"/>
-      <c r="BJ36" s="44"/>
-      <c r="BK36" s="44"/>
-      <c r="BL36" s="44"/>
+      <c r="I36" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="J36" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="K36" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="L36" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="M36" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="N36" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="O36" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="P36" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="Q36" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="R36" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="S36" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="T36" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="U36" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="V36" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="W36" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="X36" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="Y36" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="Z36" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AA36" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AB36" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AC36" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AD36" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AE36" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AF36" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AG36" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AH36" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AI36" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AJ36" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AK36" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AL36" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AM36" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AN36" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AO36" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AP36" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AQ36" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AR36" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AS36" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AT36" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AU36" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AV36" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AW36" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AX36" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AY36" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AZ36" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BA36" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BB36" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BC36" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BD36" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BE36" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BF36" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BG36" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BH36" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BI36" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BJ36" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BK36" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BL36" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BM36" s="46"/>
     </row>
-    <row r="37" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D37" s="4"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="3"/>
+    <row r="37" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="10"/>
+      <c r="B37" s="69" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="44"/>
+      <c r="K37" s="44"/>
+      <c r="L37" s="44"/>
+      <c r="M37" s="44"/>
+      <c r="N37" s="44"/>
+      <c r="O37" s="44"/>
+      <c r="P37" s="44"/>
+      <c r="Q37" s="44"/>
+      <c r="R37" s="44"/>
+      <c r="S37" s="44"/>
+      <c r="T37" s="44"/>
+      <c r="U37" s="44"/>
+      <c r="V37" s="44"/>
+      <c r="W37" s="44"/>
+      <c r="X37" s="44"/>
+      <c r="Y37" s="44"/>
+      <c r="Z37" s="44"/>
+      <c r="AA37" s="44"/>
+      <c r="AB37" s="44"/>
+      <c r="AC37" s="44"/>
+      <c r="AD37" s="44"/>
+      <c r="AE37" s="44"/>
+      <c r="AF37" s="44"/>
+      <c r="AG37" s="44"/>
+      <c r="AH37" s="44"/>
+      <c r="AI37" s="44"/>
+      <c r="AJ37" s="44"/>
+      <c r="AK37" s="44"/>
+      <c r="AL37" s="44"/>
+      <c r="AM37" s="44"/>
+      <c r="AN37" s="44"/>
+      <c r="AO37" s="44"/>
+      <c r="AP37" s="44"/>
+      <c r="AQ37" s="44"/>
+      <c r="AR37" s="44"/>
+      <c r="AS37" s="44"/>
+      <c r="AT37" s="44"/>
+      <c r="AU37" s="44"/>
+      <c r="AV37" s="44"/>
+      <c r="AW37" s="44"/>
+      <c r="AX37" s="44"/>
+      <c r="AY37" s="44"/>
+      <c r="AZ37" s="44"/>
+      <c r="BA37" s="44"/>
+      <c r="BB37" s="44"/>
+      <c r="BC37" s="44"/>
+      <c r="BD37" s="44"/>
+      <c r="BE37" s="44"/>
+      <c r="BF37" s="44"/>
+      <c r="BG37" s="44"/>
+      <c r="BH37" s="44"/>
+      <c r="BI37" s="44"/>
+      <c r="BJ37" s="44"/>
+      <c r="BK37" s="44"/>
+      <c r="BL37" s="44"/>
     </row>
     <row r="38" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D38" s="5"/>
+      <c r="D38" s="4"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D39" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -9058,7 +9056,7 @@
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="S4:V4"/>
   </mergeCells>
-  <conditionalFormatting sqref="E9:E36">
+  <conditionalFormatting sqref="E9:E37">
     <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9082,12 +9080,12 @@
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL36">
+  <conditionalFormatting sqref="I7:BL37">
     <cfRule type="expression" dxfId="11" priority="1">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10:BL35">
+  <conditionalFormatting sqref="I10:BL36">
     <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
       <formula>AND($C10="Low Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
@@ -9104,7 +9102,7 @@
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36:BL36">
+  <conditionalFormatting sqref="I37:BL37">
     <cfRule type="expression" dxfId="5" priority="13" stopIfTrue="1">
       <formula>AND(#REF!="Low Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
@@ -9130,7 +9128,7 @@
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolling Increment" prompt="Changing this number will scroll the Gantt Chart view." sqref="C7" xr:uid="{662A47A0-7258-440E-8D71-BC54CBC9C651}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C35" xr:uid="{12A8278F-D51D-4B98-A311-DB5FCD18D214}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C36" xr:uid="{12A8278F-D51D-4B98-A311-DB5FCD18D214}">
       <formula1>"Goal,Milestone,On Track, Low Risk, Med Risk, High Risk"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C11" xr:uid="{218D9212-09C8-4DA2-9014-64503951B170}">
@@ -9144,8 +9142,8 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A scrollbar is in cells I8 through BL8. _x000a_To jump forward or backward in the timeline, enter a value of 0 or higher in cell C7._x000a_A value of 0 takes you to the beginning of the chart." sqref="A8" xr:uid="{737D7247-B514-41B2-94CC-2F538E17DE66}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row contains headers for the project schedule.  B9 through G9 contains schedule information.  Cells I9 through BL9 contain the first letter of each day of the week for the date above that heading._x000a_All project timeline charting is auto generated." sqref="A9" xr:uid="{6AB925DC-9BC9-4EC3-A848-25121289EECD}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Project information starting in cell B11 through cell G11. _x000a_Enter Milestone Description, select a Category, assign someone to the task, and enter the progress, start date, and number of days for the task to start charting._x000a_" sqref="A11" xr:uid="{77315CCB-C571-42B0-8983-9C17BB04F75F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Gantt milestone data. DO NOT enter anything in this row. _x000a_To add more items, insert new rows above this one._x000a_" sqref="A36" xr:uid="{659FD5CB-B62B-4854-B8A9-29F1F70930AC}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is an empty row" sqref="A35" xr:uid="{60F6BB2A-523D-41BA-B324-85E19FB9FF7E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Gantt milestone data. DO NOT enter anything in this row. _x000a_To add more items, insert new rows above this one._x000a_" sqref="A37" xr:uid="{659FD5CB-B62B-4854-B8A9-29F1F70930AC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is an empty row" sqref="A36" xr:uid="{60F6BB2A-523D-41BA-B324-85E19FB9FF7E}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
@@ -9172,7 +9170,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E9:E36</xm:sqref>
+          <xm:sqref>E9:E37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="6" id="{39412BF5-D1E8-4731-95F6-6B0C252D35F8}">
@@ -9191,7 +9189,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>I10:BL35</xm:sqref>
+          <xm:sqref>I10:BL36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="12" id="{A1EFF969-3CBB-4DB2-A4C9-47B01FE32C86}">
@@ -9210,7 +9208,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>I36:BL36</xm:sqref>
+          <xm:sqref>I37:BL37</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -9219,23 +9217,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9539,22 +9526,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11AAADB5-F91F-44CE-8CB6-D8472D59D975}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9C5315E-9A69-4EEB-ACCD-0F886FBF12FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9581,9 +9575,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9C5315E-9A69-4EEB-ACCD-0F886FBF12FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11AAADB5-F91F-44CE-8CB6-D8472D59D975}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>